<commit_message>
Fix AV reppel issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_1_2023.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_1_2023.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,28 +429,28 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve"> </v>
+        <v>004/ZZZ</v>
       </c>
       <c r="B2" t="str">
-        <v xml:space="preserve"> </v>
+        <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v xml:space="preserve"> </v>
+        <v>IR801997</v>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve"> </v>
+        <v>NOUBAIL MOHAMMED</v>
       </c>
       <c r="E2" t="str">
-        <v xml:space="preserve"> </v>
+        <v>non</v>
       </c>
       <c r="F2" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G2" t="str">
-        <v xml:space="preserve"> </v>
+        <v>mensuelle</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -471,12 +471,106 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>004/ZZZ</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C3" t="str">
+        <v>IB19558</v>
+      </c>
+      <c r="D3" t="str">
+        <v>ZERNAKH ABDELLAH</v>
+      </c>
+      <c r="E3" t="str">
+        <v>non</v>
+      </c>
+      <c r="F3" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="B4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H4">
+        <v>2000</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>